<commit_message>
Updated the name and email column order
</commit_message>
<xml_diff>
--- a/data/contacts.xlsx
+++ b/data/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fb649a3fb494198/Documents/Python/ExcelPost/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{119D67DE-42A7-4FB6-997F-72CABEDD89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B4025BD-D2F0-4376-9C01-3B666542AC12}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{119D67DE-42A7-4FB6-997F-72CABEDD89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB703B6D-B3AF-409B-A5AC-AFAC2F6AA3ED}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11235" xr2:uid="{B655607A-835A-45A8-B577-935A26C3C1F8}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,10 +455,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -469,10 +469,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -497,10 +497,10 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -511,10 +511,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>

</xml_diff>